<commit_message>
change wrong department  name
</commit_message>
<xml_diff>
--- a/public/Excel_example/college_data.xlsx
+++ b/public/Excel_example/college_data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wang\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9150"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="103">
   <si>
     <t>文學院</t>
   </si>
@@ -121,9 +116,6 @@
   </si>
   <si>
     <t>法學院</t>
-  </si>
-  <si>
-    <t>法律系/法律所</t>
   </si>
   <si>
     <t>財經法律學系</t>
@@ -328,6 +320,14 @@
   </si>
   <si>
     <t>單位名稱部門</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>法律系法學組/法律所</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>法律系法制組/法律所</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1238,7 +1238,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1261,16 +1261,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1760,7 +1760,7 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,7 +1774,7 @@
         <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1788,7 +1788,7 @@
         <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,10 +1799,10 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,10 +1813,10 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
         <v>36</v>
-      </c>
-      <c r="D40" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,10 +1827,10 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,10 +1841,10 @@
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,10 +1855,10 @@
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,10 +1869,10 @@
         <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1883,10 +1883,10 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,10 +1897,10 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,10 +1911,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,10 +1925,10 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,10 +1939,10 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" t="s">
         <v>45</v>
-      </c>
-      <c r="D49" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,10 +1953,10 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,10 +1967,10 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,10 +1981,10 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1995,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2009,10 +2009,10 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" t="s">
         <v>50</v>
-      </c>
-      <c r="D54" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,10 +2023,10 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2037,10 +2037,10 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,10 +2051,10 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2065,10 +2065,10 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,10 +2079,10 @@
         <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,10 +2093,10 @@
         <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2107,10 +2107,10 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2121,10 +2121,10 @@
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2135,10 +2135,10 @@
         <v>10</v>
       </c>
       <c r="C63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,10 +2149,10 @@
         <v>11</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2163,10 +2163,10 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2177,10 +2177,10 @@
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2191,10 +2191,10 @@
         <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2205,10 +2205,10 @@
         <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2219,10 +2219,10 @@
         <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2233,10 +2233,10 @@
         <v>17</v>
       </c>
       <c r="C70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2247,10 +2247,10 @@
         <v>18</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2261,10 +2261,10 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2275,10 +2275,10 @@
         <v>20</v>
       </c>
       <c r="C73" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2289,10 +2289,10 @@
         <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2303,10 +2303,10 @@
         <v>22</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2317,10 +2317,10 @@
         <v>23</v>
       </c>
       <c r="C76" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2331,10 +2331,10 @@
         <v>24</v>
       </c>
       <c r="C77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2345,10 +2345,10 @@
         <v>25</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2359,10 +2359,10 @@
         <v>26</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D79" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2373,10 +2373,10 @@
         <v>27</v>
       </c>
       <c r="C80" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2387,10 +2387,10 @@
         <v>28</v>
       </c>
       <c r="C81" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D81" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2401,10 +2401,10 @@
         <v>29</v>
       </c>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2415,10 +2415,10 @@
         <v>30</v>
       </c>
       <c r="C83" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2429,10 +2429,10 @@
         <v>31</v>
       </c>
       <c r="C84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2443,10 +2443,10 @@
         <v>32</v>
       </c>
       <c r="C85" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2457,10 +2457,10 @@
         <v>33</v>
       </c>
       <c r="C86" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2471,10 +2471,10 @@
         <v>34</v>
       </c>
       <c r="C87" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2485,10 +2485,10 @@
         <v>35</v>
       </c>
       <c r="C88" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2499,10 +2499,10 @@
         <v>36</v>
       </c>
       <c r="C89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D89" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2513,10 +2513,10 @@
         <v>0</v>
       </c>
       <c r="C90" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D90" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2527,10 +2527,10 @@
         <v>0</v>
       </c>
       <c r="C91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2541,10 +2541,10 @@
         <v>0</v>
       </c>
       <c r="C92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2555,10 +2555,10 @@
         <v>0</v>
       </c>
       <c r="C93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2569,10 +2569,10 @@
         <v>0</v>
       </c>
       <c r="C94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2583,10 +2583,10 @@
         <v>0</v>
       </c>
       <c r="C95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2597,10 +2597,10 @@
         <v>0</v>
       </c>
       <c r="C96" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D96" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2611,10 +2611,10 @@
         <v>0</v>
       </c>
       <c r="C97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2625,10 +2625,10 @@
         <v>0</v>
       </c>
       <c r="C98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2639,10 +2639,10 @@
         <v>0</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2653,10 +2653,10 @@
         <v>0</v>
       </c>
       <c r="C100" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D100" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>